<commit_message>
Ordenação por seleção e inserção
</commit_message>
<xml_diff>
--- a/Estrutura de dados/TesteDeMesa.xlsx
+++ b/Estrutura de dados/TesteDeMesa.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27645" windowHeight="13125" activeTab="4"/>
+    <workbookView windowWidth="27150" windowHeight="13125" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -12,13 +12,15 @@
     <sheet name="teste2" sheetId="3" r:id="rId3"/>
     <sheet name="teste3" sheetId="4" r:id="rId4"/>
     <sheet name="teste4" sheetId="5" r:id="rId5"/>
+    <sheet name="Ordenação" sheetId="6" r:id="rId6"/>
+    <sheet name="Insercao" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="224">
   <si>
     <t>Teste de mesa 1</t>
   </si>
@@ -636,6 +638,60 @@
   </si>
   <si>
     <t>qtdMaiorMedia++;</t>
+  </si>
+  <si>
+    <t>Public ordenacao {</t>
+  </si>
+  <si>
+    <t>Passo</t>
+  </si>
+  <si>
+    <t>fila</t>
+  </si>
+  <si>
+    <t>qtdFila</t>
+  </si>
+  <si>
+    <t>j</t>
+  </si>
+  <si>
+    <t>[50,54,82,62,74,99,61,52,64,89,58]</t>
+  </si>
+  <si>
+    <t>private int[] fila = [50,54,82,62,74,99,61,52,64,89,58]</t>
+  </si>
+  <si>
+    <t>int qtdFila = fila.lenght() - 1;</t>
+  </si>
+  <si>
+    <t>for(int i = qtdFila; i &gt; 0; i--){</t>
+  </si>
+  <si>
+    <t>int j;</t>
+  </si>
+  <si>
+    <t>for( int j = 0; j &lt;= i; j++){</t>
+  </si>
+  <si>
+    <t>if(fila[i] &gt; fila[maior]){</t>
+  </si>
+  <si>
+    <t>maior = i;</t>
+  </si>
+  <si>
+    <t>int troca = fila[maior];</t>
+  </si>
+  <si>
+    <t>fila[maior] = fila [j-1];</t>
+  </si>
+  <si>
+    <t>fila[j-1] = troca;</t>
+  </si>
+  <si>
+    <t>maior = 0;</t>
+  </si>
+  <si>
+    <t>troca</t>
   </si>
 </sst>
 </file>
@@ -643,9 +699,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="22">
@@ -680,6 +736,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
@@ -690,43 +753,6 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -744,6 +770,35 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -767,21 +822,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -794,15 +835,30 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -816,7 +872,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -825,49 +881,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -885,6 +911,120 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -897,13 +1037,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -915,67 +1055,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -987,25 +1073,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1106,17 +1174,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1177,6 +1239,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -1185,121 +1262,112 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -1308,31 +1376,31 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1342,8 +1410,18 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -1728,1400 +1806,1400 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6">
-      <c r="B2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
+      <c r="B2" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
     </row>
     <row r="3" spans="2:6">
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="2:6">
-      <c r="B4" s="5">
+      <c r="B4" s="11">
         <v>1</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="12">
         <v>10</v>
       </c>
-      <c r="E4" s="6">
-        <v>0</v>
-      </c>
-      <c r="F4" s="6">
+      <c r="E4" s="12">
+        <v>0</v>
+      </c>
+      <c r="F4" s="12">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="2:6">
-      <c r="B5" s="5">
+      <c r="B5" s="11">
         <v>2</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="12">
         <v>10</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="12">
         <v>20</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="12">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="2:6">
-      <c r="B6" s="5">
+      <c r="B6" s="11">
         <v>3</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="12">
         <v>10</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="12">
         <v>20</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F6" s="12">
         <v>10</v>
       </c>
     </row>
     <row r="7" spans="2:6">
-      <c r="B7" s="5">
+      <c r="B7" s="11">
         <v>4</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="12">
         <v>20</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="12">
         <v>20</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F7" s="12">
         <v>10</v>
       </c>
     </row>
     <row r="8" spans="2:6">
-      <c r="B8" s="5">
+      <c r="B8" s="11">
         <v>5</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="12">
         <v>20</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="12">
         <v>10</v>
       </c>
-      <c r="F8" s="6">
+      <c r="F8" s="12">
         <v>10</v>
       </c>
     </row>
     <row r="9" spans="2:6">
-      <c r="B9" s="5">
+      <c r="B9" s="11">
         <v>6</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="12">
         <v>20</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="12">
         <v>10</v>
       </c>
-      <c r="F9" s="6">
+      <c r="F9" s="12">
         <v>10</v>
       </c>
     </row>
     <row r="11" spans="2:4">
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="8"/>
-      <c r="D11" s="9"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="15"/>
     </row>
     <row r="12" spans="2:4">
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="10" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="13" spans="2:4">
-      <c r="B13" s="5">
+      <c r="B13" s="11">
         <v>1</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="6">
+      <c r="D13" s="12">
         <v>100</v>
       </c>
     </row>
     <row r="14" spans="2:4">
-      <c r="B14" s="5">
+      <c r="B14" s="11">
         <v>2</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="6">
+      <c r="D14" s="12">
         <v>99</v>
       </c>
     </row>
     <row r="16" spans="2:6">
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
     </row>
     <row r="17" spans="2:6">
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D17" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="E17" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="F17" s="4" t="s">
+      <c r="F17" s="10" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="18" spans="2:6">
-      <c r="B18" s="5">
+      <c r="B18" s="11">
         <v>1</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="D18" s="6">
+      <c r="D18" s="12">
         <v>20</v>
       </c>
-      <c r="E18" s="6">
-        <v>0</v>
-      </c>
-      <c r="F18" s="6">
+      <c r="E18" s="12">
+        <v>0</v>
+      </c>
+      <c r="F18" s="12">
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="2:6">
-      <c r="B19" s="5">
+      <c r="B19" s="11">
         <v>2</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="D19" s="6">
+      <c r="D19" s="12">
         <v>20</v>
       </c>
-      <c r="E19" s="6">
+      <c r="E19" s="12">
         <v>10</v>
       </c>
-      <c r="F19" s="6">
+      <c r="F19" s="12">
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="2:6">
-      <c r="B20" s="5">
+      <c r="B20" s="11">
         <v>3</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C20" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D20" s="6">
+      <c r="D20" s="12">
         <v>20</v>
       </c>
-      <c r="E20" s="6">
+      <c r="E20" s="12">
         <v>10</v>
       </c>
-      <c r="F20" s="6">
+      <c r="F20" s="12">
         <v>200</v>
       </c>
     </row>
     <row r="21" spans="2:6">
-      <c r="B21" s="5">
+      <c r="B21" s="11">
         <v>4</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="C21" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="D21" s="6">
+      <c r="D21" s="12">
         <v>20</v>
       </c>
-      <c r="E21" s="6">
+      <c r="E21" s="12">
         <v>10</v>
       </c>
-      <c r="F21" s="6">
+      <c r="F21" s="12">
         <v>200</v>
       </c>
     </row>
     <row r="23" spans="2:7">
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10"/>
     </row>
     <row r="24" spans="2:7">
-      <c r="B24" s="4" t="s">
+      <c r="B24" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C24" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D24" s="4" t="s">
+      <c r="D24" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="E24" s="4" t="s">
+      <c r="E24" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="F24" s="4" t="s">
+      <c r="F24" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="G24" s="4" t="s">
+      <c r="G24" s="10" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="25" spans="2:7">
-      <c r="B25" s="5">
+      <c r="B25" s="11">
         <v>1</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="C25" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="D25" s="6">
+      <c r="D25" s="12">
         <v>23</v>
       </c>
-      <c r="E25" s="6">
-        <v>0</v>
-      </c>
-      <c r="F25" s="6">
-        <v>0</v>
-      </c>
-      <c r="G25" s="6">
+      <c r="E25" s="12">
+        <v>0</v>
+      </c>
+      <c r="F25" s="12">
+        <v>0</v>
+      </c>
+      <c r="G25" s="12">
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="2:7">
-      <c r="B26" s="5">
+      <c r="B26" s="11">
         <v>2</v>
       </c>
-      <c r="C26" s="6" t="s">
+      <c r="C26" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="D26" s="6">
+      <c r="D26" s="12">
         <v>23</v>
       </c>
-      <c r="E26" s="6">
+      <c r="E26" s="12">
         <v>4</v>
       </c>
-      <c r="F26" s="6">
-        <v>0</v>
-      </c>
-      <c r="G26" s="6">
+      <c r="F26" s="12">
+        <v>0</v>
+      </c>
+      <c r="G26" s="12">
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="2:7">
-      <c r="B27" s="5">
+      <c r="B27" s="11">
         <v>3</v>
       </c>
-      <c r="C27" s="6" t="s">
+      <c r="C27" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="D27" s="6">
+      <c r="D27" s="12">
         <v>23</v>
       </c>
-      <c r="E27" s="6">
+      <c r="E27" s="12">
         <v>4</v>
       </c>
-      <c r="F27" s="6">
+      <c r="F27" s="12">
         <v>20</v>
       </c>
-      <c r="G27" s="6">
+      <c r="G27" s="12">
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="2:7">
-      <c r="B28" s="5">
+      <c r="B28" s="11">
         <v>4</v>
       </c>
-      <c r="C28" s="6" t="s">
+      <c r="C28" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="D28" s="6">
+      <c r="D28" s="12">
         <v>23</v>
       </c>
-      <c r="E28" s="6">
+      <c r="E28" s="12">
         <v>4</v>
       </c>
-      <c r="F28" s="6">
+      <c r="F28" s="12">
         <v>20</v>
       </c>
-      <c r="G28" s="6">
+      <c r="G28" s="12">
         <v>8535</v>
       </c>
     </row>
     <row r="29" spans="2:7">
-      <c r="B29" s="5">
+      <c r="B29" s="11">
         <v>5</v>
       </c>
-      <c r="C29" s="6" t="s">
+      <c r="C29" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="D29" s="6">
+      <c r="D29" s="12">
         <v>23</v>
       </c>
-      <c r="E29" s="6">
+      <c r="E29" s="12">
         <v>4</v>
       </c>
-      <c r="F29" s="6">
+      <c r="F29" s="12">
         <v>20</v>
       </c>
-      <c r="G29" s="6">
+      <c r="G29" s="12">
         <v>8535</v>
       </c>
     </row>
     <row r="31" spans="2:10">
-      <c r="B31" s="4" t="s">
+      <c r="B31" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
-      <c r="F31" s="4"/>
-      <c r="G31" s="4"/>
-      <c r="H31" s="4"/>
-      <c r="I31" s="4"/>
-      <c r="J31" s="4"/>
+      <c r="C31" s="10"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="10"/>
+      <c r="F31" s="10"/>
+      <c r="G31" s="10"/>
+      <c r="H31" s="10"/>
+      <c r="I31" s="10"/>
+      <c r="J31" s="10"/>
     </row>
     <row r="32" spans="2:10">
-      <c r="B32" s="4" t="s">
+      <c r="B32" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C32" s="4" t="s">
+      <c r="C32" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D32" s="4" t="s">
+      <c r="D32" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="E32" s="4" t="s">
+      <c r="E32" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="F32" s="4" t="s">
+      <c r="F32" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="G32" s="4" t="s">
+      <c r="G32" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="H32" s="17" t="s">
+      <c r="H32" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="I32" s="17" t="s">
+      <c r="I32" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="J32" s="17" t="s">
+      <c r="J32" s="23" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="33" spans="2:10">
-      <c r="B33" s="10">
+      <c r="B33" s="16">
         <v>1</v>
       </c>
-      <c r="C33" s="11" t="s">
+      <c r="C33" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="D33" s="12">
+      <c r="D33" s="18">
         <v>1000</v>
       </c>
-      <c r="E33" s="12">
-        <v>0</v>
-      </c>
-      <c r="F33" s="12">
-        <v>0</v>
-      </c>
-      <c r="G33" s="12">
-        <v>0</v>
-      </c>
-      <c r="H33" s="13">
-        <v>0</v>
-      </c>
-      <c r="I33" s="13">
-        <v>0</v>
-      </c>
-      <c r="J33" s="13">
+      <c r="E33" s="18">
+        <v>0</v>
+      </c>
+      <c r="F33" s="18">
+        <v>0</v>
+      </c>
+      <c r="G33" s="18">
+        <v>0</v>
+      </c>
+      <c r="H33" s="19">
+        <v>0</v>
+      </c>
+      <c r="I33" s="19">
+        <v>0</v>
+      </c>
+      <c r="J33" s="19">
         <v>0</v>
       </c>
     </row>
     <row r="34" spans="2:10">
-      <c r="B34" s="5">
+      <c r="B34" s="11">
         <v>2</v>
       </c>
-      <c r="C34" s="6" t="s">
+      <c r="C34" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="D34" s="13">
+      <c r="D34" s="19">
         <v>1000</v>
       </c>
-      <c r="E34" s="13">
+      <c r="E34" s="19">
         <v>500</v>
       </c>
-      <c r="F34" s="13">
-        <v>0</v>
-      </c>
-      <c r="G34" s="13">
-        <v>0</v>
-      </c>
-      <c r="H34" s="13">
-        <v>0</v>
-      </c>
-      <c r="I34" s="13">
-        <v>0</v>
-      </c>
-      <c r="J34" s="13">
+      <c r="F34" s="19">
+        <v>0</v>
+      </c>
+      <c r="G34" s="19">
+        <v>0</v>
+      </c>
+      <c r="H34" s="19">
+        <v>0</v>
+      </c>
+      <c r="I34" s="19">
+        <v>0</v>
+      </c>
+      <c r="J34" s="19">
         <v>0</v>
       </c>
     </row>
     <row r="35" spans="2:10">
-      <c r="B35" s="5">
+      <c r="B35" s="11">
         <v>3</v>
       </c>
-      <c r="C35" s="6" t="s">
+      <c r="C35" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="D35" s="13">
+      <c r="D35" s="19">
         <v>1000</v>
       </c>
-      <c r="E35" s="13">
+      <c r="E35" s="19">
         <v>500</v>
       </c>
-      <c r="F35" s="13">
-        <v>200</v>
-      </c>
-      <c r="G35" s="13">
-        <v>0</v>
-      </c>
-      <c r="H35" s="13">
-        <v>0</v>
-      </c>
-      <c r="I35" s="13">
-        <v>0</v>
-      </c>
-      <c r="J35" s="13">
+      <c r="F35" s="19">
+        <v>200</v>
+      </c>
+      <c r="G35" s="19">
+        <v>0</v>
+      </c>
+      <c r="H35" s="19">
+        <v>0</v>
+      </c>
+      <c r="I35" s="19">
+        <v>0</v>
+      </c>
+      <c r="J35" s="19">
         <v>0</v>
       </c>
     </row>
     <row r="36" spans="2:10">
-      <c r="B36" s="5">
+      <c r="B36" s="11">
         <v>4</v>
       </c>
-      <c r="C36" s="6" t="s">
+      <c r="C36" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="D36" s="13">
+      <c r="D36" s="19">
         <v>1000</v>
       </c>
-      <c r="E36" s="13">
+      <c r="E36" s="19">
         <v>500</v>
       </c>
-      <c r="F36" s="13">
-        <v>200</v>
-      </c>
-      <c r="G36" s="13">
+      <c r="F36" s="19">
+        <v>200</v>
+      </c>
+      <c r="G36" s="19">
         <v>300</v>
       </c>
-      <c r="H36" s="13">
-        <v>0</v>
-      </c>
-      <c r="I36" s="13">
-        <v>0</v>
-      </c>
-      <c r="J36" s="13">
+      <c r="H36" s="19">
+        <v>0</v>
+      </c>
+      <c r="I36" s="19">
+        <v>0</v>
+      </c>
+      <c r="J36" s="19">
         <v>0</v>
       </c>
     </row>
     <row r="37" spans="2:10">
-      <c r="B37" s="5">
+      <c r="B37" s="11">
         <v>5</v>
       </c>
-      <c r="C37" s="6" t="s">
+      <c r="C37" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="D37" s="13">
+      <c r="D37" s="19">
         <v>1000</v>
       </c>
-      <c r="E37" s="13">
+      <c r="E37" s="19">
         <v>500</v>
       </c>
-      <c r="F37" s="13">
-        <v>200</v>
-      </c>
-      <c r="G37" s="13">
+      <c r="F37" s="19">
+        <v>200</v>
+      </c>
+      <c r="G37" s="19">
         <v>300</v>
       </c>
-      <c r="H37" s="13">
+      <c r="H37" s="19">
         <v>30</v>
       </c>
-      <c r="I37" s="13">
-        <v>0</v>
-      </c>
-      <c r="J37" s="13">
+      <c r="I37" s="19">
+        <v>0</v>
+      </c>
+      <c r="J37" s="19">
         <v>0</v>
       </c>
     </row>
     <row r="38" spans="2:10">
-      <c r="B38" s="5">
+      <c r="B38" s="11">
         <v>6</v>
       </c>
-      <c r="C38" s="6" t="s">
+      <c r="C38" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="D38" s="13">
+      <c r="D38" s="19">
         <v>1000</v>
       </c>
-      <c r="E38" s="13">
+      <c r="E38" s="19">
         <v>500</v>
       </c>
-      <c r="F38" s="13">
-        <v>200</v>
-      </c>
-      <c r="G38" s="13">
+      <c r="F38" s="19">
+        <v>200</v>
+      </c>
+      <c r="G38" s="19">
         <v>300</v>
       </c>
-      <c r="H38" s="13">
+      <c r="H38" s="19">
         <v>30</v>
       </c>
-      <c r="I38" s="13">
+      <c r="I38" s="19">
         <v>50</v>
       </c>
-      <c r="J38" s="13">
+      <c r="J38" s="19">
         <v>0</v>
       </c>
     </row>
     <row r="39" spans="2:10">
-      <c r="B39" s="5">
+      <c r="B39" s="11">
         <v>7</v>
       </c>
-      <c r="C39" s="6" t="s">
+      <c r="C39" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="D39" s="13">
+      <c r="D39" s="19">
         <v>1000</v>
       </c>
-      <c r="E39" s="13">
+      <c r="E39" s="19">
         <v>500</v>
       </c>
-      <c r="F39" s="13">
-        <v>200</v>
-      </c>
-      <c r="G39" s="13">
+      <c r="F39" s="19">
+        <v>200</v>
+      </c>
+      <c r="G39" s="19">
         <v>300</v>
       </c>
-      <c r="H39" s="13">
+      <c r="H39" s="19">
         <v>30</v>
       </c>
-      <c r="I39" s="13">
+      <c r="I39" s="19">
         <v>50</v>
       </c>
-      <c r="J39" s="13">
+      <c r="J39" s="19">
         <v>20</v>
       </c>
     </row>
     <row r="40" spans="2:10">
-      <c r="B40" s="5">
+      <c r="B40" s="11">
         <v>8</v>
       </c>
-      <c r="C40" s="14" t="s">
+      <c r="C40" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="D40" s="15">
+      <c r="D40" s="21">
         <v>1000</v>
       </c>
-      <c r="E40" s="15">
+      <c r="E40" s="21">
         <v>500</v>
       </c>
-      <c r="F40" s="15">
-        <v>200</v>
-      </c>
-      <c r="G40" s="15">
+      <c r="F40" s="21">
+        <v>200</v>
+      </c>
+      <c r="G40" s="21">
         <v>300</v>
       </c>
-      <c r="H40" s="15">
+      <c r="H40" s="21">
         <v>30</v>
       </c>
-      <c r="I40" s="15">
+      <c r="I40" s="21">
         <v>50</v>
       </c>
-      <c r="J40" s="15">
+      <c r="J40" s="21">
         <v>20</v>
       </c>
     </row>
     <row r="41" spans="2:10">
-      <c r="B41" s="5"/>
-      <c r="C41" s="14"/>
-      <c r="D41" s="10">
+      <c r="B41" s="11"/>
+      <c r="C41" s="20"/>
+      <c r="D41" s="16">
         <v>1000</v>
       </c>
-      <c r="E41" s="10">
+      <c r="E41" s="16">
         <v>500</v>
       </c>
-      <c r="F41" s="10">
-        <v>200</v>
-      </c>
-      <c r="G41" s="10">
+      <c r="F41" s="16">
+        <v>200</v>
+      </c>
+      <c r="G41" s="16">
         <v>300</v>
       </c>
-      <c r="H41" s="10">
+      <c r="H41" s="16">
         <v>30</v>
       </c>
-      <c r="I41" s="10">
+      <c r="I41" s="16">
         <v>50</v>
       </c>
-      <c r="J41" s="10">
+      <c r="J41" s="16">
         <v>20</v>
       </c>
     </row>
     <row r="43" spans="2:6">
-      <c r="B43" s="4" t="s">
+      <c r="B43" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="C43" s="4"/>
-      <c r="D43" s="4"/>
-      <c r="E43" s="4"/>
-      <c r="F43" s="4"/>
+      <c r="C43" s="10"/>
+      <c r="D43" s="10"/>
+      <c r="E43" s="10"/>
+      <c r="F43" s="10"/>
     </row>
     <row r="44" spans="2:6">
-      <c r="B44" s="4" t="s">
+      <c r="B44" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C44" s="4" t="s">
+      <c r="C44" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D44" s="4" t="s">
+      <c r="D44" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="E44" s="4" t="s">
+      <c r="E44" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="F44" s="4" t="s">
+      <c r="F44" s="10" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="45" spans="2:6">
-      <c r="B45" s="5">
+      <c r="B45" s="11">
         <v>1</v>
       </c>
-      <c r="C45" s="6" t="s">
+      <c r="C45" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="D45" s="6">
+      <c r="D45" s="12">
         <v>1741</v>
       </c>
-      <c r="E45" s="6">
-        <v>0</v>
-      </c>
-      <c r="F45" s="6">
+      <c r="E45" s="12">
+        <v>0</v>
+      </c>
+      <c r="F45" s="12">
         <v>0</v>
       </c>
     </row>
     <row r="46" spans="2:6">
-      <c r="B46" s="5">
+      <c r="B46" s="11">
         <v>2</v>
       </c>
-      <c r="C46" s="6" t="s">
+      <c r="C46" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="D46" s="6">
+      <c r="D46" s="12">
         <v>1741</v>
       </c>
-      <c r="E46" s="6">
+      <c r="E46" s="12">
         <v>4</v>
       </c>
-      <c r="F46" s="6">
+      <c r="F46" s="12">
         <v>0</v>
       </c>
     </row>
     <row r="47" spans="2:6">
-      <c r="B47" s="5">
+      <c r="B47" s="11">
         <v>3</v>
       </c>
-      <c r="C47" s="6" t="s">
+      <c r="C47" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="D47" s="6">
+      <c r="D47" s="12">
         <v>1741</v>
       </c>
-      <c r="E47" s="6">
+      <c r="E47" s="12">
         <v>4</v>
       </c>
-      <c r="F47" s="6">
+      <c r="F47" s="12">
         <v>1810.64</v>
       </c>
     </row>
     <row r="48" spans="2:6">
-      <c r="B48" s="5">
+      <c r="B48" s="11">
         <v>4</v>
       </c>
-      <c r="C48" s="6" t="s">
+      <c r="C48" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="D48" s="6">
+      <c r="D48" s="12">
         <v>1741</v>
       </c>
-      <c r="E48" s="6">
+      <c r="E48" s="12">
         <v>4</v>
       </c>
-      <c r="F48" s="6">
+      <c r="F48" s="12">
         <v>1810.64</v>
       </c>
     </row>
     <row r="50" spans="2:5">
-      <c r="B50" s="7" t="s">
+      <c r="B50" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="C50" s="8"/>
-      <c r="D50" s="8"/>
-      <c r="E50" s="9"/>
+      <c r="C50" s="14"/>
+      <c r="D50" s="14"/>
+      <c r="E50" s="15"/>
     </row>
     <row r="51" spans="2:5">
-      <c r="B51" s="4" t="s">
+      <c r="B51" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C51" s="4" t="s">
+      <c r="C51" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D51" s="4" t="s">
+      <c r="D51" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="E51" s="4" t="s">
+      <c r="E51" s="10" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="52" spans="2:5">
-      <c r="B52" s="5">
+      <c r="B52" s="11">
         <v>1</v>
       </c>
-      <c r="C52" s="6" t="s">
+      <c r="C52" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="D52" s="6">
+      <c r="D52" s="12">
         <v>22000</v>
       </c>
-      <c r="E52" s="6">
+      <c r="E52" s="12">
         <v>0</v>
       </c>
     </row>
     <row r="53" spans="2:5">
-      <c r="B53" s="5">
+      <c r="B53" s="11">
         <v>2</v>
       </c>
-      <c r="C53" s="6" t="s">
+      <c r="C53" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="D53" s="6">
+      <c r="D53" s="12">
         <v>22000</v>
       </c>
-      <c r="E53" s="6">
+      <c r="E53" s="12">
         <v>38060</v>
       </c>
     </row>
     <row r="54" spans="2:5">
-      <c r="B54" s="5">
+      <c r="B54" s="11">
         <v>3</v>
       </c>
-      <c r="C54" s="6" t="s">
+      <c r="C54" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="D54" s="6">
+      <c r="D54" s="12">
         <v>22000</v>
       </c>
-      <c r="E54" s="6">
+      <c r="E54" s="12">
         <v>38060</v>
       </c>
     </row>
     <row r="56" spans="2:9">
-      <c r="B56" s="7" t="s">
+      <c r="B56" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="C56" s="8"/>
-      <c r="D56" s="8"/>
-      <c r="E56" s="8"/>
-      <c r="F56" s="8"/>
-      <c r="G56" s="8"/>
-      <c r="H56" s="8"/>
-      <c r="I56" s="9"/>
+      <c r="C56" s="14"/>
+      <c r="D56" s="14"/>
+      <c r="E56" s="14"/>
+      <c r="F56" s="14"/>
+      <c r="G56" s="14"/>
+      <c r="H56" s="14"/>
+      <c r="I56" s="15"/>
     </row>
     <row r="57" spans="2:9">
-      <c r="B57" s="16" t="s">
+      <c r="B57" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C57" s="16" t="s">
+      <c r="C57" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="D57" s="16" t="s">
+      <c r="D57" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="E57" s="16" t="s">
+      <c r="E57" s="22" t="s">
         <v>65</v>
       </c>
-      <c r="F57" s="16" t="s">
+      <c r="F57" s="22" t="s">
         <v>66</v>
       </c>
-      <c r="G57" s="16" t="s">
+      <c r="G57" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="H57" s="18" t="s">
+      <c r="H57" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="I57" s="6" t="s">
+      <c r="I57" s="12" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="58" spans="2:9">
-      <c r="B58" s="10">
+      <c r="B58" s="16">
         <v>1</v>
       </c>
-      <c r="C58" s="11" t="s">
+      <c r="C58" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="D58" s="12">
-        <v>0</v>
-      </c>
-      <c r="E58" s="12">
-        <v>0</v>
-      </c>
-      <c r="F58" s="12">
-        <v>0</v>
-      </c>
-      <c r="G58" s="12">
-        <v>0</v>
-      </c>
-      <c r="H58" s="13">
-        <v>0</v>
-      </c>
-      <c r="I58" s="6" t="s">
+      <c r="D58" s="18">
+        <v>0</v>
+      </c>
+      <c r="E58" s="18">
+        <v>0</v>
+      </c>
+      <c r="F58" s="18">
+        <v>0</v>
+      </c>
+      <c r="G58" s="18">
+        <v>0</v>
+      </c>
+      <c r="H58" s="19">
+        <v>0</v>
+      </c>
+      <c r="I58" s="12" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="59" spans="2:9">
-      <c r="B59" s="5">
+      <c r="B59" s="11">
         <v>2</v>
       </c>
-      <c r="C59" s="11" t="s">
+      <c r="C59" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="D59" s="13">
-        <v>0</v>
-      </c>
-      <c r="E59" s="13">
-        <v>0</v>
-      </c>
-      <c r="F59" s="13">
-        <v>0</v>
-      </c>
-      <c r="G59" s="13">
+      <c r="D59" s="19">
+        <v>0</v>
+      </c>
+      <c r="E59" s="19">
+        <v>0</v>
+      </c>
+      <c r="F59" s="19">
+        <v>0</v>
+      </c>
+      <c r="G59" s="19">
         <v>1741</v>
       </c>
-      <c r="H59" s="13">
-        <v>0</v>
-      </c>
-      <c r="I59" s="6" t="s">
+      <c r="H59" s="19">
+        <v>0</v>
+      </c>
+      <c r="I59" s="12" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="60" spans="2:9">
-      <c r="B60" s="5">
+      <c r="B60" s="11">
         <v>3</v>
       </c>
-      <c r="C60" s="6" t="s">
+      <c r="C60" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="D60" s="13">
-        <v>0</v>
-      </c>
-      <c r="E60" s="13">
+      <c r="D60" s="19">
+        <v>0</v>
+      </c>
+      <c r="E60" s="19">
         <v>10</v>
       </c>
-      <c r="F60" s="13">
-        <v>0</v>
-      </c>
-      <c r="G60" s="13">
+      <c r="F60" s="19">
+        <v>0</v>
+      </c>
+      <c r="G60" s="19">
         <v>1741</v>
       </c>
-      <c r="H60" s="13">
-        <v>0</v>
-      </c>
-      <c r="I60" s="6" t="s">
+      <c r="H60" s="19">
+        <v>0</v>
+      </c>
+      <c r="I60" s="12" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="61" spans="2:9">
-      <c r="B61" s="5">
+      <c r="B61" s="11">
         <v>4</v>
       </c>
-      <c r="C61" s="6" t="s">
+      <c r="C61" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="D61" s="13">
-        <v>0</v>
-      </c>
-      <c r="E61" s="13">
+      <c r="D61" s="19">
+        <v>0</v>
+      </c>
+      <c r="E61" s="19">
         <v>10</v>
       </c>
-      <c r="F61" s="13">
+      <c r="F61" s="19">
         <v>500</v>
       </c>
-      <c r="G61" s="13">
+      <c r="G61" s="19">
         <v>1741</v>
       </c>
-      <c r="H61" s="13">
-        <v>0</v>
-      </c>
-      <c r="I61" s="6" t="s">
+      <c r="H61" s="19">
+        <v>0</v>
+      </c>
+      <c r="I61" s="12" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="62" spans="2:9">
-      <c r="B62" s="5">
+      <c r="B62" s="11">
         <v>5</v>
       </c>
-      <c r="C62" s="6" t="s">
+      <c r="C62" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="D62" s="13">
-        <v>200</v>
-      </c>
-      <c r="E62" s="13">
+      <c r="D62" s="19">
+        <v>200</v>
+      </c>
+      <c r="E62" s="19">
         <v>10</v>
       </c>
-      <c r="F62" s="13">
+      <c r="F62" s="19">
         <v>500</v>
       </c>
-      <c r="G62" s="13">
+      <c r="G62" s="19">
         <v>1741</v>
       </c>
-      <c r="H62" s="13">
-        <v>0</v>
-      </c>
-      <c r="I62" s="6" t="s">
+      <c r="H62" s="19">
+        <v>0</v>
+      </c>
+      <c r="I62" s="12" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="63" spans="2:9">
-      <c r="B63" s="5">
+      <c r="B63" s="11">
         <v>6</v>
       </c>
-      <c r="C63" s="6" t="s">
+      <c r="C63" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="D63" s="13">
-        <v>200</v>
-      </c>
-      <c r="E63" s="13">
+      <c r="D63" s="19">
+        <v>200</v>
+      </c>
+      <c r="E63" s="19">
         <v>10</v>
       </c>
-      <c r="F63" s="13">
+      <c r="F63" s="19">
         <v>500</v>
       </c>
-      <c r="G63" s="13">
+      <c r="G63" s="19">
         <v>1741</v>
       </c>
-      <c r="H63" s="13">
+      <c r="H63" s="19">
         <v>3766</v>
       </c>
-      <c r="I63" s="6" t="s">
+      <c r="I63" s="12" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="64" spans="2:9">
-      <c r="B64" s="5">
+      <c r="B64" s="11">
         <v>7</v>
       </c>
-      <c r="C64" s="6" t="s">
+      <c r="C64" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="D64" s="13">
-        <v>200</v>
-      </c>
-      <c r="E64" s="13">
+      <c r="D64" s="19">
+        <v>200</v>
+      </c>
+      <c r="E64" s="19">
         <v>10</v>
       </c>
-      <c r="F64" s="13">
+      <c r="F64" s="19">
         <v>500</v>
       </c>
-      <c r="G64" s="13">
+      <c r="G64" s="19">
         <v>1741</v>
       </c>
-      <c r="H64" s="13">
+      <c r="H64" s="19">
         <v>3766</v>
       </c>
-      <c r="I64" s="6" t="s">
+      <c r="I64" s="12" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="66" spans="2:5">
-      <c r="B66" s="7" t="s">
+      <c r="B66" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="C66" s="8"/>
-      <c r="D66" s="8"/>
-      <c r="E66" s="9"/>
+      <c r="C66" s="14"/>
+      <c r="D66" s="14"/>
+      <c r="E66" s="15"/>
     </row>
     <row r="67" spans="2:5">
-      <c r="B67" s="4" t="s">
+      <c r="B67" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C67" s="4" t="s">
+      <c r="C67" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D67" s="4" t="s">
+      <c r="D67" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="E67" s="4" t="s">
+      <c r="E67" s="10" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="68" ht="25.5" spans="2:5">
-      <c r="B68" s="5">
+      <c r="B68" s="11">
         <v>1</v>
       </c>
-      <c r="C68" s="19" t="s">
+      <c r="C68" s="25" t="s">
         <v>81</v>
       </c>
-      <c r="D68" s="5">
+      <c r="D68" s="11">
         <v>33</v>
       </c>
-      <c r="E68" s="5">
+      <c r="E68" s="11">
         <v>0</v>
       </c>
     </row>
     <row r="69" ht="25.5" spans="2:5">
-      <c r="B69" s="5">
+      <c r="B69" s="11">
         <v>2</v>
       </c>
-      <c r="C69" s="19" t="s">
+      <c r="C69" s="25" t="s">
         <v>82</v>
       </c>
-      <c r="D69" s="5">
+      <c r="D69" s="11">
         <v>33</v>
       </c>
-      <c r="E69" s="5">
+      <c r="E69" s="11">
         <v>91.4</v>
       </c>
     </row>
     <row r="71" spans="2:5">
-      <c r="B71" s="7" t="s">
+      <c r="B71" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="C71" s="8"/>
-      <c r="D71" s="8"/>
-      <c r="E71" s="9"/>
+      <c r="C71" s="14"/>
+      <c r="D71" s="14"/>
+      <c r="E71" s="15"/>
     </row>
     <row r="72" spans="2:5">
-      <c r="B72" s="4" t="s">
+      <c r="B72" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C72" s="4" t="s">
+      <c r="C72" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D72" s="4" t="s">
+      <c r="D72" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="E72" s="4" t="s">
+      <c r="E72" s="10" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="73" spans="2:5">
-      <c r="B73" s="5">
+      <c r="B73" s="11">
         <v>1</v>
       </c>
-      <c r="C73" s="19" t="s">
+      <c r="C73" s="25" t="s">
         <v>86</v>
       </c>
-      <c r="D73" s="5">
-        <v>0</v>
-      </c>
-      <c r="E73" s="5">
+      <c r="D73" s="11">
+        <v>0</v>
+      </c>
+      <c r="E73" s="11">
         <v>0</v>
       </c>
     </row>
     <row r="74" spans="2:5">
-      <c r="B74" s="5">
+      <c r="B74" s="11">
         <v>2</v>
       </c>
-      <c r="C74" s="19" t="s">
+      <c r="C74" s="25" t="s">
         <v>87</v>
       </c>
-      <c r="D74" s="5">
-        <v>0</v>
-      </c>
-      <c r="E74" s="5">
+      <c r="D74" s="11">
+        <v>0</v>
+      </c>
+      <c r="E74" s="11">
         <v>0</v>
       </c>
     </row>
     <row r="75" spans="2:5">
-      <c r="B75" s="5">
+      <c r="B75" s="11">
         <v>3</v>
       </c>
-      <c r="C75" s="19" t="s">
+      <c r="C75" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="D75" s="5">
-        <v>0</v>
-      </c>
-      <c r="E75" s="5">
+      <c r="D75" s="11">
+        <v>0</v>
+      </c>
+      <c r="E75" s="11">
         <v>11</v>
       </c>
     </row>
     <row r="76" spans="2:5">
-      <c r="B76" s="5">
+      <c r="B76" s="11">
         <v>4</v>
       </c>
-      <c r="C76" s="19" t="s">
+      <c r="C76" s="25" t="s">
         <v>89</v>
       </c>
-      <c r="D76" s="5" t="s">
+      <c r="D76" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="E76" s="5">
+      <c r="E76" s="11">
         <v>11</v>
       </c>
     </row>
     <row r="77" spans="2:5">
-      <c r="B77" s="5">
+      <c r="B77" s="11">
         <v>5</v>
       </c>
-      <c r="C77" s="19" t="s">
+      <c r="C77" s="25" t="s">
         <v>91</v>
       </c>
-      <c r="D77" s="5">
-        <v>0</v>
-      </c>
-      <c r="E77" s="5">
+      <c r="D77" s="11">
+        <v>0</v>
+      </c>
+      <c r="E77" s="11">
         <v>0</v>
       </c>
     </row>
     <row r="79" spans="2:6">
-      <c r="B79" s="6" t="s">
+      <c r="B79" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C79" s="6" t="s">
+      <c r="C79" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="D79" s="6" t="s">
+      <c r="D79" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="E79" s="6" t="s">
+      <c r="E79" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="F79" s="6" t="s">
+      <c r="F79" s="12" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="80" spans="2:6">
-      <c r="B80" s="6">
+      <c r="B80" s="12">
         <v>1</v>
       </c>
-      <c r="C80" s="6" t="s">
+      <c r="C80" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="D80" s="6" t="s">
+      <c r="D80" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="E80" s="6" t="s">
+      <c r="E80" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="F80" s="6">
+      <c r="F80" s="12">
         <v>0</v>
       </c>
     </row>
     <row r="81" spans="2:6">
-      <c r="B81" s="6">
+      <c r="B81" s="12">
         <v>2</v>
       </c>
-      <c r="C81" s="6" t="s">
+      <c r="C81" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="D81" s="6" t="s">
+      <c r="D81" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="E81" s="6" t="s">
+      <c r="E81" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="F81" s="6">
+      <c r="F81" s="12">
         <v>0</v>
       </c>
     </row>
     <row r="82" spans="2:6">
-      <c r="B82" s="6">
+      <c r="B82" s="12">
         <v>3</v>
       </c>
-      <c r="C82" s="6" t="s">
+      <c r="C82" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="D82" s="6" t="s">
+      <c r="D82" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="E82" s="6" t="s">
+      <c r="E82" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="F82" s="6">
+      <c r="F82" s="12">
         <v>0</v>
       </c>
     </row>
     <row r="83" spans="2:6">
-      <c r="B83" s="6">
+      <c r="B83" s="12">
         <v>4</v>
       </c>
-      <c r="C83" s="6" t="s">
+      <c r="C83" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="D83" s="6" t="s">
+      <c r="D83" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="E83" s="6" t="s">
+      <c r="E83" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="F83" s="6">
+      <c r="F83" s="12">
         <v>0</v>
       </c>
     </row>
     <row r="84" spans="2:6">
-      <c r="B84" s="6">
+      <c r="B84" s="12">
         <v>5</v>
       </c>
-      <c r="C84" s="6" t="s">
+      <c r="C84" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="D84" s="6" t="s">
+      <c r="D84" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="E84" s="6" t="s">
+      <c r="E84" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="F84" s="6">
+      <c r="F84" s="12">
         <v>0</v>
       </c>
     </row>
     <row r="85" spans="2:6">
-      <c r="B85" s="6">
+      <c r="B85" s="12">
         <v>6</v>
       </c>
-      <c r="C85" s="6" t="s">
+      <c r="C85" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="D85" s="6" t="s">
+      <c r="D85" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="E85" s="6" t="s">
+      <c r="E85" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="F85" s="6">
+      <c r="F85" s="12">
         <v>0</v>
       </c>
     </row>
     <row r="86" spans="2:6">
-      <c r="B86" s="6">
+      <c r="B86" s="12">
         <v>7</v>
       </c>
-      <c r="C86" s="6" t="s">
+      <c r="C86" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="D86" s="6" t="s">
+      <c r="D86" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="E86" s="6" t="s">
+      <c r="E86" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="F86" s="6">
+      <c r="F86" s="12">
         <v>0</v>
       </c>
     </row>
     <row r="87" spans="2:6">
-      <c r="B87" s="6" t="s">
+      <c r="B87" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="C87" s="6" t="s">
+      <c r="C87" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="D87" s="6" t="s">
+      <c r="D87" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="E87" s="6" t="s">
+      <c r="E87" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="F87" s="6" t="s">
+      <c r="F87" s="12" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="88" spans="2:6">
-      <c r="B88" s="6">
+      <c r="B88" s="12">
         <v>15</v>
       </c>
-      <c r="C88" s="6" t="s">
+      <c r="C88" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="D88" s="6" t="s">
+      <c r="D88" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="E88" s="6" t="s">
+      <c r="E88" s="12" t="s">
         <v>113</v>
       </c>
-      <c r="F88" s="6">
+      <c r="F88" s="12">
         <v>0</v>
       </c>
     </row>
     <row r="89" spans="2:6">
-      <c r="B89" s="6">
+      <c r="B89" s="12">
         <v>16</v>
       </c>
-      <c r="C89" s="6" t="s">
+      <c r="C89" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="D89" s="6" t="s">
+      <c r="D89" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="E89" s="6" t="s">
+      <c r="E89" s="12" t="s">
         <v>113</v>
       </c>
-      <c r="F89" s="6">
+      <c r="F89" s="12">
         <v>4</v>
       </c>
     </row>
@@ -3195,7 +3273,7 @@
       <c r="C3">
         <v>0</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="9" t="s">
         <v>121</v>
       </c>
       <c r="E3">
@@ -3215,7 +3293,7 @@
       <c r="C4">
         <v>1</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="9" t="s">
         <v>121</v>
       </c>
       <c r="E4">
@@ -3235,7 +3313,7 @@
       <c r="C5">
         <v>2</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="9" t="s">
         <v>121</v>
       </c>
       <c r="E5">
@@ -3255,7 +3333,7 @@
       <c r="C6">
         <v>3</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="9" t="s">
         <v>121</v>
       </c>
       <c r="E6">
@@ -3275,7 +3353,7 @@
       <c r="C7">
         <v>4</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="9" t="s">
         <v>121</v>
       </c>
       <c r="E7">
@@ -3295,7 +3373,7 @@
       <c r="C8">
         <v>5</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="9" t="s">
         <v>121</v>
       </c>
       <c r="E8">
@@ -3309,13 +3387,13 @@
       </c>
     </row>
     <row r="9" spans="2:10">
-      <c r="B9" s="3">
+      <c r="B9" s="9">
         <v>7</v>
       </c>
       <c r="C9">
         <v>6</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="9" t="s">
         <v>121</v>
       </c>
       <c r="E9">
@@ -3329,35 +3407,35 @@
       </c>
     </row>
     <row r="10" spans="2:11">
-      <c r="B10" s="3"/>
-      <c r="D10" s="3"/>
+      <c r="B10" s="9"/>
+      <c r="D10" s="9"/>
       <c r="K10" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="11" spans="2:12">
-      <c r="B11" s="3"/>
-      <c r="D11" s="3"/>
+      <c r="B11" s="9"/>
+      <c r="D11" s="9"/>
       <c r="L11" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="12" spans="2:12">
-      <c r="B12" s="3"/>
-      <c r="D12" s="3"/>
+      <c r="B12" s="9"/>
+      <c r="D12" s="9"/>
       <c r="L12" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="13" spans="2:4">
-      <c r="B13" s="3"/>
-      <c r="D13" s="3"/>
+      <c r="B13" s="9"/>
+      <c r="D13" s="9"/>
     </row>
     <row r="14" spans="2:2">
-      <c r="B14" s="3"/>
+      <c r="B14" s="9"/>
     </row>
     <row r="15" spans="2:2">
-      <c r="B15" s="3"/>
+      <c r="B15" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3431,8 +3509,8 @@
       <c r="C4">
         <v>1</v>
       </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
       <c r="F4">
         <v>20</v>
       </c>
@@ -3450,8 +3528,8 @@
       <c r="C5">
         <v>2</v>
       </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
       <c r="F5">
         <v>20</v>
       </c>
@@ -3469,7 +3547,7 @@
       <c r="C6">
         <v>3</v>
       </c>
-      <c r="E6" s="3"/>
+      <c r="E6" s="9"/>
       <c r="F6">
         <v>20</v>
       </c>
@@ -3487,8 +3565,8 @@
       <c r="C7">
         <v>0</v>
       </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
       <c r="F7">
         <v>30</v>
       </c>
@@ -3506,8 +3584,8 @@
       <c r="C8">
         <v>1</v>
       </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3" t="s">
+      <c r="D8" s="9"/>
+      <c r="E8" s="9" t="s">
         <v>141</v>
       </c>
       <c r="F8">
@@ -3527,8 +3605,8 @@
       <c r="C9">
         <v>2</v>
       </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
       <c r="F9">
         <v>25</v>
       </c>
@@ -3546,7 +3624,7 @@
       <c r="C10">
         <v>3</v>
       </c>
-      <c r="E10" s="3"/>
+      <c r="E10" s="9"/>
       <c r="F10">
         <v>25</v>
       </c>
@@ -3567,7 +3645,7 @@
       <c r="D11" t="s">
         <v>144</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="E11" s="9" t="s">
         <v>145</v>
       </c>
       <c r="F11">
@@ -3767,7 +3845,7 @@
       </c>
     </row>
     <row r="24" spans="4:4">
-      <c r="D24" s="1"/>
+      <c r="D24" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3927,7 +4005,7 @@
       <c r="I9">
         <v>3</v>
       </c>
-      <c r="L9" s="2" t="s">
+      <c r="L9" s="8" t="s">
         <v>170</v>
       </c>
     </row>
@@ -4111,7 +4189,7 @@
   <sheetPr/>
   <dimension ref="A1:P49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="L40" sqref="L8:L40"/>
     </sheetView>
   </sheetViews>
@@ -4122,7 +4200,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="7" t="s">
         <v>171</v>
       </c>
     </row>
@@ -4140,7 +4218,7 @@
       </c>
     </row>
     <row r="4" spans="1:15">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="7" t="s">
         <v>174</v>
       </c>
       <c r="O4" t="s">
@@ -4476,7 +4554,7 @@
       <c r="D16">
         <v>8</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="E16" s="7" t="s">
         <v>196</v>
       </c>
       <c r="F16">
@@ -5591,6 +5669,733 @@
       </c>
       <c r="L49">
         <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="C3:O21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D49" sqref="D49"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="12.75"/>
+  <cols>
+    <col min="4" max="4" width="31.3" customWidth="1"/>
+    <col min="5" max="5" width="6.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="11:11">
+      <c r="K3" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="4" spans="3:8">
+      <c r="C4" t="s">
+        <v>207</v>
+      </c>
+      <c r="D4" t="s">
+        <v>208</v>
+      </c>
+      <c r="E4" t="s">
+        <v>209</v>
+      </c>
+      <c r="F4" t="s">
+        <v>116</v>
+      </c>
+      <c r="G4" t="s">
+        <v>210</v>
+      </c>
+      <c r="H4" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="5" spans="3:12">
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="E5" s="1">
+        <v>10</v>
+      </c>
+      <c r="F5">
+        <v>10</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="L5" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="6" spans="3:8">
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="3:12">
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="G7">
+        <v>2</v>
+      </c>
+      <c r="H7">
+        <v>2</v>
+      </c>
+      <c r="L7" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="8" spans="3:12">
+      <c r="C8">
+        <v>4</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="G8">
+        <v>3</v>
+      </c>
+      <c r="H8" t="s">
+        <v>169</v>
+      </c>
+      <c r="L8" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="9" spans="3:8">
+      <c r="C9">
+        <v>5</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="G9">
+        <v>4</v>
+      </c>
+      <c r="H9" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="10" spans="3:12">
+      <c r="C10">
+        <v>6</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="G10">
+        <v>5</v>
+      </c>
+      <c r="H10">
+        <v>5</v>
+      </c>
+      <c r="L10" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="11" spans="3:13">
+      <c r="C11">
+        <v>7</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="G11">
+        <v>6</v>
+      </c>
+      <c r="H11" t="s">
+        <v>169</v>
+      </c>
+      <c r="M11" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="12" spans="3:13">
+      <c r="C12">
+        <v>8</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="G12">
+        <v>7</v>
+      </c>
+      <c r="H12" t="s">
+        <v>169</v>
+      </c>
+      <c r="M12" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="13" spans="3:14">
+      <c r="C13">
+        <v>9</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="G13">
+        <v>8</v>
+      </c>
+      <c r="H13" t="s">
+        <v>169</v>
+      </c>
+      <c r="N13" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="14" spans="3:15">
+      <c r="C14">
+        <v>10</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="G14">
+        <v>9</v>
+      </c>
+      <c r="H14" t="s">
+        <v>169</v>
+      </c>
+      <c r="O14" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="15" spans="3:14">
+      <c r="C15">
+        <v>11</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="G15">
+        <v>10</v>
+      </c>
+      <c r="N15" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="16" spans="13:13">
+      <c r="M16" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="17" spans="13:13">
+      <c r="M17" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="18" spans="13:13">
+      <c r="M18" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="19" spans="13:13">
+      <c r="M19" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="20" spans="13:13">
+      <c r="M20" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="21" spans="11:11">
+      <c r="K21" t="s">
+        <v>170</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="B2:R20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="12.75"/>
+  <cols>
+    <col min="3" max="5" width="8.8" style="1"/>
+    <col min="8" max="18" width="3.3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="8:18">
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>2</v>
+      </c>
+      <c r="K2">
+        <v>3</v>
+      </c>
+      <c r="L2">
+        <v>4</v>
+      </c>
+      <c r="M2">
+        <v>5</v>
+      </c>
+      <c r="N2">
+        <v>6</v>
+      </c>
+      <c r="O2">
+        <v>7</v>
+      </c>
+      <c r="P2">
+        <v>8</v>
+      </c>
+      <c r="Q2">
+        <v>9</v>
+      </c>
+      <c r="R2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="2:18">
+      <c r="B3" t="s">
+        <v>207</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="H3" s="2">
+        <v>50</v>
+      </c>
+      <c r="I3" s="3">
+        <v>54</v>
+      </c>
+      <c r="J3" s="3">
+        <v>82</v>
+      </c>
+      <c r="K3" s="3">
+        <v>62</v>
+      </c>
+      <c r="L3" s="3">
+        <v>74</v>
+      </c>
+      <c r="M3" s="3">
+        <v>99</v>
+      </c>
+      <c r="N3" s="3">
+        <v>61</v>
+      </c>
+      <c r="O3" s="3">
+        <v>52</v>
+      </c>
+      <c r="P3" s="3">
+        <v>64</v>
+      </c>
+      <c r="Q3" s="3">
+        <v>89</v>
+      </c>
+      <c r="R3" s="3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="2:18">
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1">
+        <v>-1</v>
+      </c>
+      <c r="H4" s="3">
+        <v>50</v>
+      </c>
+      <c r="I4" s="3">
+        <v>54</v>
+      </c>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="3"/>
+    </row>
+    <row r="5" spans="2:18">
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5" s="1">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0</v>
+      </c>
+      <c r="H5" s="3">
+        <v>50</v>
+      </c>
+      <c r="I5" s="3">
+        <v>54</v>
+      </c>
+      <c r="J5" s="3">
+        <v>82</v>
+      </c>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="3"/>
+      <c r="R5" s="3"/>
+    </row>
+    <row r="6" spans="2:18">
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6" s="1">
+        <v>2</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1</v>
+      </c>
+      <c r="H6" s="3">
+        <v>50</v>
+      </c>
+      <c r="I6" s="3">
+        <v>54</v>
+      </c>
+      <c r="J6" s="4">
+        <v>62</v>
+      </c>
+      <c r="K6" s="4">
+        <v>82</v>
+      </c>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="3"/>
+    </row>
+    <row r="7" spans="2:18">
+      <c r="B7">
+        <v>4</v>
+      </c>
+      <c r="C7" s="1">
+        <v>3</v>
+      </c>
+      <c r="D7" s="1">
+        <v>2</v>
+      </c>
+      <c r="E7" s="1">
+        <v>62</v>
+      </c>
+      <c r="H7" s="3">
+        <v>50</v>
+      </c>
+      <c r="I7" s="3">
+        <v>54</v>
+      </c>
+      <c r="J7" s="3">
+        <v>62</v>
+      </c>
+      <c r="K7" s="4">
+        <v>74</v>
+      </c>
+      <c r="L7" s="4">
+        <v>82</v>
+      </c>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="3"/>
+      <c r="R7" s="3"/>
+    </row>
+    <row r="8" spans="2:13">
+      <c r="B8">
+        <v>5</v>
+      </c>
+      <c r="C8" s="1">
+        <v>3</v>
+      </c>
+      <c r="D8" s="1">
+        <v>1</v>
+      </c>
+      <c r="H8" s="3">
+        <v>50</v>
+      </c>
+      <c r="I8" s="3">
+        <v>54</v>
+      </c>
+      <c r="J8" s="3">
+        <v>62</v>
+      </c>
+      <c r="K8" s="5">
+        <v>74</v>
+      </c>
+      <c r="L8" s="5">
+        <v>82</v>
+      </c>
+      <c r="M8" s="6">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14">
+      <c r="B9">
+        <v>6</v>
+      </c>
+      <c r="C9" s="1">
+        <v>4</v>
+      </c>
+      <c r="D9" s="1">
+        <v>3</v>
+      </c>
+      <c r="H9">
+        <v>50</v>
+      </c>
+      <c r="I9">
+        <v>54</v>
+      </c>
+      <c r="J9" s="6">
+        <v>61</v>
+      </c>
+      <c r="K9" s="6">
+        <v>62</v>
+      </c>
+      <c r="L9" s="6">
+        <v>74</v>
+      </c>
+      <c r="M9" s="6">
+        <v>82</v>
+      </c>
+      <c r="N9" s="6">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4">
+      <c r="B10">
+        <v>7</v>
+      </c>
+      <c r="C10" s="1">
+        <v>4</v>
+      </c>
+      <c r="D10" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4">
+      <c r="B11">
+        <v>8</v>
+      </c>
+      <c r="C11" s="1">
+        <v>4</v>
+      </c>
+      <c r="D11" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4">
+      <c r="B12">
+        <v>9</v>
+      </c>
+      <c r="C12" s="1">
+        <v>5</v>
+      </c>
+      <c r="D12" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4">
+      <c r="B13">
+        <v>10</v>
+      </c>
+      <c r="C13" s="1">
+        <v>5</v>
+      </c>
+      <c r="D13" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4">
+      <c r="B14">
+        <v>11</v>
+      </c>
+      <c r="C14" s="1">
+        <v>5</v>
+      </c>
+      <c r="D14" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4">
+      <c r="B15">
+        <v>12</v>
+      </c>
+      <c r="C15" s="1">
+        <v>5</v>
+      </c>
+      <c r="D15" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5">
+      <c r="B16">
+        <v>13</v>
+      </c>
+      <c r="C16" s="1">
+        <v>6</v>
+      </c>
+      <c r="D16" s="1">
+        <v>5</v>
+      </c>
+      <c r="E16" s="1">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4">
+      <c r="B17">
+        <v>14</v>
+      </c>
+      <c r="C17" s="1">
+        <v>6</v>
+      </c>
+      <c r="D17" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4">
+      <c r="B18">
+        <v>15</v>
+      </c>
+      <c r="C18" s="1">
+        <v>6</v>
+      </c>
+      <c r="D18" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4">
+      <c r="B19">
+        <v>16</v>
+      </c>
+      <c r="C19" s="1">
+        <v>6</v>
+      </c>
+      <c r="D19" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4">
+      <c r="B20">
+        <v>17</v>
+      </c>
+      <c r="C20" s="1">
+        <v>6</v>
+      </c>
+      <c r="D20" s="1">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>